<commit_message>
updated grade for leon
</commit_message>
<xml_diff>
--- a/Rev1 Final Presentation Rubric.xlsx
+++ b/Rev1 Final Presentation Rubric.xlsx
@@ -327,11 +327,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +550,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -562,12 +562,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>49</v>
       </c>
       <c r="F1" s="2"/>
@@ -596,16 +596,16 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="17">
-        <v>0.85</v>
+      <c r="C2" s="16"/>
+      <c r="D2" s="14">
+        <v>0.95</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="13">
         <f>D2*B42</f>
-        <v>68.424999999999997</v>
+        <v>76.474999999999994</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -633,14 +633,14 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="17">
+      <c r="C3" s="16"/>
+      <c r="D3" s="14">
         <v>0.85</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <f>D3*B42</f>
         <v>68.424999999999997</v>
       </c>
@@ -670,14 +670,14 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17">
+      <c r="C4" s="16"/>
+      <c r="D4" s="14">
         <v>1.05</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <f>D4*B42</f>
         <v>84.525000000000006</v>
       </c>

</xml_diff>